<commit_message>
Added some poster resources
</commit_message>
<xml_diff>
--- a/Investigation/deeper_chatbot_experiments/experiment_results.xlsx
+++ b/Investigation/deeper_chatbot_experiments/experiment_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nathan\Documents\GitHub\Individual-Project\Investigation\deeper_chatbot_experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04891A3D-49B6-4546-AA35-797AE5EE17A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8F1373C-4B2C-4CF2-AF6F-49FE3F294CBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Bot/tech</t>
   </si>
@@ -39,9 +39,6 @@
     <t>cost</t>
   </si>
   <si>
-    <t>extendibility</t>
-  </si>
-  <si>
     <t>time to respond - echo</t>
   </si>
   <si>
@@ -64,6 +61,39 @@
   </si>
   <si>
     <t>Free</t>
+  </si>
+  <si>
+    <t>Instantly</t>
+  </si>
+  <si>
+    <t>$19/month + $9/channel</t>
+  </si>
+  <si>
+    <t>With paid version</t>
+  </si>
+  <si>
+    <t>All - with paid version</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>extendibile</t>
+  </si>
+  <si>
+    <t>$0.007 per message, + other google cloud platform costs</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>other features?</t>
+  </si>
+  <si>
+    <t>Designed for speech to text requests</t>
+  </si>
+  <si>
+    <t>Industry standard</t>
   </si>
 </sst>
 </file>
@@ -381,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -394,18 +424,19 @@
     <col min="3" max="3" width="27.28515625" customWidth="1"/>
     <col min="4" max="4" width="20.7109375" customWidth="1"/>
     <col min="5" max="5" width="15.7109375" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" customWidth="1"/>
+    <col min="6" max="6" width="50.28515625" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
         <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -417,31 +448,67 @@
         <v>3</v>
       </c>
       <c r="G1" t="s">
-        <v>4</v>
+        <v>17</v>
+      </c>
+      <c r="H1" t="s">
+        <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
         <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>